<commit_message>
更新phyFa os code size
</commit_message>
<xml_diff>
--- a/RTOS_core_codesize.xlsx
+++ b/RTOS_core_codesize.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0E09F85F-F19F-43F7-8EA8-7909763C5E79}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Release_X2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,13 +38,33 @@
   </si>
   <si>
     <t>EC80,               60.544Bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phyfa.OS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS.lib code size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,992Bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OAL(OSA)code size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30,032Bytes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,44 +393,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{0B2E9177-9525-4D22-AA61-FE871693D756}"/>
+    <hyperlink ref="C5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>